<commit_message>
Update Christmas holidays for Berlin.
</commit_message>
<xml_diff>
--- a/src/original_data/vacations/vacations_2020.xlsx
+++ b/src/original_data/vacations/vacations_2020.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="101">
   <si>
     <t xml:space="preserve">Bundesland</t>
   </si>
@@ -106,16 +106,19 @@
     <t xml:space="preserve">12.10.2020 - 24.10.2020</t>
   </si>
   <si>
+    <t xml:space="preserve">21.12.2020 – 10.01.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01.02.2021 - 06.02.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brandenburg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.06.2020 - 08.08.2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">21.12.2020 - 02.01.2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01.02.2021 - 06.02.2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brandenburg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.06.2020 - 08.08.2020</t>
   </si>
   <si>
     <t xml:space="preserve">29.03.2021 - 09.04.2021</t>
@@ -428,10 +431,10 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="32.66"/>
@@ -566,169 +569,169 @@
         <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>29</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>21</v>
@@ -736,140 +739,140 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>20</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>10</v>
@@ -878,16 +881,16 @@
         <v>25</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Fix typo in vacations.
</commit_message>
<xml_diff>
--- a/src/original_data/vacations/vacations_2020.xlsx
+++ b/src/original_data/vacations/vacations_2020.xlsx
@@ -106,7 +106,7 @@
     <t xml:space="preserve">12.10.2020 - 24.10.2020</t>
   </si>
   <si>
-    <t xml:space="preserve">21.12.2020 – 10.01.2021</t>
+    <t xml:space="preserve">21.12.2020 - 10.01.2021</t>
   </si>
   <si>
     <t xml:space="preserve">01.02.2021 - 06.02.2021</t>
@@ -430,11 +430,11 @@
   </sheetPr>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="32.66"/>

</xml_diff>

<commit_message>
Changes for the Christmas report and general improvements.
</commit_message>
<xml_diff>
--- a/src/original_data/vacations/vacations_2020.xlsx
+++ b/src/original_data/vacations/vacations_2020.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="101">
   <si>
     <t xml:space="preserve">Bundesland</t>
   </si>
@@ -106,16 +106,19 @@
     <t xml:space="preserve">12.10.2020 - 24.10.2020</t>
   </si>
   <si>
+    <t xml:space="preserve">21.12.2020 - 10.01.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01.02.2021 - 06.02.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brandenburg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.06.2020 - 08.08.2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">21.12.2020 - 02.01.2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01.02.2021 - 06.02.2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brandenburg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.06.2020 - 08.08.2020</t>
   </si>
   <si>
     <t xml:space="preserve">29.03.2021 - 09.04.2021</t>
@@ -427,11 +430,11 @@
   </sheetPr>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="32.66"/>
@@ -566,169 +569,169 @@
         <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>29</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>21</v>
@@ -736,140 +739,140 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>20</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>10</v>
@@ -878,16 +881,16 @@
         <v>25</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Switch to English federal state names.
</commit_message>
<xml_diff>
--- a/src/original_data/vacations/vacations_2020.xlsx
+++ b/src/original_data/vacations/vacations_2020.xlsx
@@ -82,7 +82,7 @@
     <t xml:space="preserve">29.07.2021 - 11.09.2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Bayern</t>
+    <t xml:space="preserve">Bavaria</t>
   </si>
   <si>
     <t xml:space="preserve">24.02.2020 - 28.02.2020</t>
@@ -259,7 +259,7 @@
     <t xml:space="preserve">21.06.2021 - 31.07.2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Niedersachsen</t>
+    <t xml:space="preserve">Lower Saxony</t>
   </si>
   <si>
     <t xml:space="preserve">30.03.2020 - 14.04.2020</t>
@@ -268,7 +268,7 @@
     <t xml:space="preserve">12.10.2020 - 23.10.2020</t>
   </si>
   <si>
-    <t xml:space="preserve">Nordrhein-Westfalen</t>
+    <t xml:space="preserve">North Rhine-Westphalia</t>
   </si>
   <si>
     <t xml:space="preserve">29.06.2020 - 11.08.2020</t>
@@ -283,7 +283,7 @@
     <t xml:space="preserve">05.07.2021 - 17.08.2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Rheinland-Pfalz</t>
+    <t xml:space="preserve">Rhineland-Palatinate</t>
   </si>
   <si>
     <t xml:space="preserve">17.02.2020 - 21.02.2020</t>
@@ -310,7 +310,7 @@
     <t xml:space="preserve">25.05.2021 - 28.05.2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Sachsen</t>
+    <t xml:space="preserve">Saxony</t>
   </si>
   <si>
     <t xml:space="preserve">10.02.2020 - 22.02.2020</t>
@@ -334,7 +334,7 @@
     <t xml:space="preserve">26.07.2021 - 03.09.2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Sachsen-Anhalt</t>
+    <t xml:space="preserve">Saxony-Anhalt</t>
   </si>
   <si>
     <t xml:space="preserve">10.02.2020 - 14.02.2020</t>
@@ -379,7 +379,7 @@
     <t xml:space="preserve">14.05.2021 - 15.05.2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Thüringen</t>
+    <t xml:space="preserve">Thuringia</t>
   </si>
   <si>
     <t xml:space="preserve">20.07.2020 - 29.08.2020</t>
@@ -514,10 +514,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="K17" activeCellId="0" sqref="K17"/>
+      <selection pane="topRight" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="2" width="32.66"/>

</xml_diff>

<commit_message>
Implement state specific work multipliers (#20)
</commit_message>
<xml_diff>
--- a/src/original_data/vacations/vacations_2020.xlsx
+++ b/src/original_data/vacations/vacations_2020.xlsx
@@ -82,7 +82,7 @@
     <t xml:space="preserve">29.07.2021 - 11.09.2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Bayern</t>
+    <t xml:space="preserve">Bavaria</t>
   </si>
   <si>
     <t xml:space="preserve">24.02.2020 - 28.02.2020</t>
@@ -259,7 +259,7 @@
     <t xml:space="preserve">21.06.2021 - 31.07.2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Niedersachsen</t>
+    <t xml:space="preserve">Lower Saxony</t>
   </si>
   <si>
     <t xml:space="preserve">30.03.2020 - 14.04.2020</t>
@@ -268,7 +268,7 @@
     <t xml:space="preserve">12.10.2020 - 23.10.2020</t>
   </si>
   <si>
-    <t xml:space="preserve">Nordrhein-Westfalen</t>
+    <t xml:space="preserve">North Rhine-Westphalia</t>
   </si>
   <si>
     <t xml:space="preserve">29.06.2020 - 11.08.2020</t>
@@ -283,7 +283,7 @@
     <t xml:space="preserve">05.07.2021 - 17.08.2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Rheinland-Pfalz</t>
+    <t xml:space="preserve">Rhineland-Palatinate</t>
   </si>
   <si>
     <t xml:space="preserve">17.02.2020 - 21.02.2020</t>
@@ -310,7 +310,7 @@
     <t xml:space="preserve">25.05.2021 - 28.05.2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Sachsen</t>
+    <t xml:space="preserve">Saxony</t>
   </si>
   <si>
     <t xml:space="preserve">10.02.2020 - 22.02.2020</t>
@@ -334,7 +334,7 @@
     <t xml:space="preserve">26.07.2021 - 03.09.2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Sachsen-Anhalt</t>
+    <t xml:space="preserve">Saxony-Anhalt</t>
   </si>
   <si>
     <t xml:space="preserve">10.02.2020 - 14.02.2020</t>
@@ -379,7 +379,7 @@
     <t xml:space="preserve">14.05.2021 - 15.05.2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Thüringen</t>
+    <t xml:space="preserve">Thuringia</t>
   </si>
   <si>
     <t xml:space="preserve">20.07.2020 - 29.08.2020</t>
@@ -514,10 +514,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="K17" activeCellId="0" sqref="K17"/>
+      <selection pane="topRight" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="2" width="32.66"/>

</xml_diff>

<commit_message>
Change holidays to exclude Hamburg from the opening of schools in the last February week.
</commit_message>
<xml_diff>
--- a/src/original_data/vacations/vacations_2020.xlsx
+++ b/src/original_data/vacations/vacations_2020.xlsx
@@ -202,7 +202,7 @@
     <t xml:space="preserve">29.01.2021</t>
   </si>
   <si>
-    <t xml:space="preserve">01.03.2021 - 12.03.2021</t>
+    <t xml:space="preserve">20.02.2021 - 12.03.2021</t>
   </si>
   <si>
     <t xml:space="preserve">10.05.2021 - 14.05.2021</t>
@@ -514,10 +514,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H20" activeCellId="0" sqref="H20"/>
+      <selection pane="topRight" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="2" width="32.66"/>

</xml_diff>

<commit_message>
Use ARS data in the simulations. Update policies to current political situation. Generalize A/B schooling and adjust policy interface. Automatically download google mobility data. Add and prepare vaccination data.
</commit_message>
<xml_diff>
--- a/src/original_data/vacations/vacations_2020.xlsx
+++ b/src/original_data/vacations/vacations_2020.xlsx
@@ -202,7 +202,7 @@
     <t xml:space="preserve">29.01.2021</t>
   </si>
   <si>
-    <t xml:space="preserve">01.03.2021 - 12.03.2021</t>
+    <t xml:space="preserve">20.02.2021 - 12.03.2021</t>
   </si>
   <si>
     <t xml:space="preserve">10.05.2021 - 14.05.2021</t>
@@ -514,10 +514,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H20" activeCellId="0" sqref="H20"/>
+      <selection pane="topRight" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="2" width="32.66"/>

</xml_diff>